<commit_message>
Corriendo todas las imp y empezando base imputada
</commit_message>
<xml_diff>
--- a/data_management/management/4. income imputation/output/VEN_income_imputation.xlsx
+++ b/data_management/management/4. income imputation/output/VEN_income_imputation.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="153">
   <si>
     <t>Employed individuals that reported they did not know if they received labor income</t>
   </si>
@@ -43413,7 +43413,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
@@ -43431,10 +43431,10 @@
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -43453,16 +43453,18 @@
       <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="B3"/>
+      <c r="C3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="8">
-        <v>26.721763085399449</v>
+        <v>33.27163350300787</v>
       </c>
       <c r="C4" s="8">
-        <v>30.434782608695656</v>
+        <v>54.54545454545454</v>
       </c>
       <c r="D4" s="8">
         <v>40.316205533596836</v>
@@ -43479,10 +43481,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="8">
-        <v>73.278236914600541</v>
+        <v>66.728366496992138</v>
       </c>
       <c r="C5" s="8">
-        <v>69.565217391304344</v>
+        <v>45.454545454545453</v>
       </c>
       <c r="D5" s="8">
         <v>59.683794466403164</v>
@@ -43509,10 +43511,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.82644628099173556</v>
+        <v>0.37019898195279966</v>
       </c>
       <c r="C7" s="8">
-        <v>0.68649885583524028</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D7" s="8">
         <v>1.1857707509881421</v>
@@ -43529,10 +43531,10 @@
         <v>15</v>
       </c>
       <c r="B8" s="8">
-        <v>11.570247933884298</v>
+        <v>12.447940768162887</v>
       </c>
       <c r="C8" s="8">
-        <v>14.187643020594965</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8">
         <v>16.600790513833992</v>
@@ -43549,10 +43551,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="8">
-        <v>31.955922865013775</v>
+        <v>22.073114298935678</v>
       </c>
       <c r="C9" s="8">
-        <v>29.977116704805489</v>
+        <v>0</v>
       </c>
       <c r="D9" s="8">
         <v>24.505928853754941</v>
@@ -43569,10 +43571,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="8">
-        <v>24.517906336088156</v>
+        <v>23.183711244794079</v>
       </c>
       <c r="C10" s="8">
-        <v>22.196796338672769</v>
+        <v>1.2121212121212122</v>
       </c>
       <c r="D10" s="8">
         <v>18.181818181818183</v>
@@ -43589,10 +43591,10 @@
         <v>18</v>
       </c>
       <c r="B11" s="8">
-        <v>18.181818181818183</v>
+        <v>20.546043498380378</v>
       </c>
       <c r="C11" s="8">
-        <v>18.077803203661329</v>
+        <v>4.8484848484848486</v>
       </c>
       <c r="D11" s="8">
         <v>21.343873517786559</v>
@@ -43609,10 +43611,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="8">
-        <v>10.192837465564738</v>
+        <v>14.669134659879685</v>
       </c>
       <c r="C12" s="8">
-        <v>12.356979405034325</v>
+        <v>39.393939393939391</v>
       </c>
       <c r="D12" s="8">
         <v>14.624505928853754</v>
@@ -43629,10 +43631,10 @@
         <v>20</v>
       </c>
       <c r="B13" s="8">
-        <v>2.7548209366391188</v>
+        <v>6.7098565478944936</v>
       </c>
       <c r="C13" s="8">
-        <v>2.5171624713958809</v>
+        <v>53.939393939393945</v>
       </c>
       <c r="D13" s="8">
         <v>3.5573122529644272</v>
@@ -43659,10 +43661,10 @@
         <v>26</v>
       </c>
       <c r="B15" s="8">
-        <v>31.680440771349861</v>
+        <v>23.553910226746876</v>
       </c>
       <c r="C15" s="8">
-        <v>32.951945080091534</v>
+        <v>38.787878787878789</v>
       </c>
       <c r="D15" s="8">
         <v>29.249011857707508</v>
@@ -43679,10 +43681,10 @@
         <v>28</v>
       </c>
       <c r="B16" s="8">
-        <v>22.314049586776861</v>
+        <v>32.993984266543272</v>
       </c>
       <c r="C16" s="8">
-        <v>27.002288329519452</v>
+        <v>15.151515151515152</v>
       </c>
       <c r="D16" s="8">
         <v>23.320158102766801</v>
@@ -43699,10 +43701,10 @@
         <v>29</v>
       </c>
       <c r="B17" s="8">
-        <v>9.9173553719008272</v>
+        <v>29.477093937991672</v>
       </c>
       <c r="C17" s="8">
-        <v>8.9244851258581246</v>
+        <v>9.6969696969696972</v>
       </c>
       <c r="D17" s="8">
         <v>8.3003952569169961</v>
@@ -43719,10 +43721,10 @@
         <v>30</v>
       </c>
       <c r="B18" s="8">
-        <v>1.3774104683195594</v>
+        <v>11.059694585839889</v>
       </c>
       <c r="C18" s="8">
-        <v>0.45766590389016021</v>
+        <v>12.121212121212121</v>
       </c>
       <c r="D18" s="8">
         <v>1.5810276679841897</v>
@@ -43739,10 +43741,10 @@
         <v>27</v>
       </c>
       <c r="B19" s="8">
-        <v>34.159779614325068</v>
+        <v>2.7764923646459971</v>
       </c>
       <c r="C19" s="8">
-        <v>30.205949656750576</v>
+        <v>23.636363636363637</v>
       </c>
       <c r="D19" s="8">
         <v>37.549407114624508</v>
@@ -43759,10 +43761,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="8">
-        <v>0.55096418732782371</v>
+        <v>0.13882461823229986</v>
       </c>
       <c r="C20" s="8">
-        <v>0.45766590389016021</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D20" s="8">
         <v>0</v>
@@ -43789,10 +43791,10 @@
         <v>33</v>
       </c>
       <c r="B22" s="8">
-        <v>3.3057851239669422</v>
+        <v>0.32392410920869968</v>
       </c>
       <c r="C22" s="8">
-        <v>2.0594965675057209</v>
+        <v>0</v>
       </c>
       <c r="D22" s="8">
         <v>0</v>
@@ -43809,10 +43811,10 @@
         <v>34</v>
       </c>
       <c r="B23" s="8">
-        <v>0</v>
+        <v>0.13882461823229986</v>
       </c>
       <c r="C23" s="8">
-        <v>0.2288329519450801</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D23" s="8">
         <v>0</v>
@@ -43829,10 +43831,10 @@
         <v>35</v>
       </c>
       <c r="B24" s="8">
-        <v>15.977961432506888</v>
+        <v>26.330402591392875</v>
       </c>
       <c r="C24" s="8">
-        <v>16.933638443935926</v>
+        <v>50.303030303030305</v>
       </c>
       <c r="D24" s="8">
         <v>11.857707509881422</v>
@@ -43849,10 +43851,10 @@
         <v>36</v>
       </c>
       <c r="B25" s="8">
-        <v>42.424242424242422</v>
+        <v>47.107820453493751</v>
       </c>
       <c r="C25" s="8">
-        <v>40.274599542334094</v>
+        <v>23.030303030303031</v>
       </c>
       <c r="D25" s="8">
         <v>42.292490118577078</v>
@@ -43869,10 +43871,10 @@
         <v>37</v>
       </c>
       <c r="B26" s="8">
-        <v>11.84573002754821</v>
+        <v>5.876908838500694</v>
       </c>
       <c r="C26" s="8">
-        <v>8.9244851258581246</v>
+        <v>7.878787878787878</v>
       </c>
       <c r="D26" s="8">
         <v>9.0909090909090917</v>
@@ -43889,10 +43891,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="8">
-        <v>21.212121212121211</v>
+        <v>14.854234150856085</v>
       </c>
       <c r="C27" s="8">
-        <v>28.375286041189931</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="D27" s="8">
         <v>20.948616600790515</v>
@@ -43909,10 +43911,10 @@
         <v>39</v>
       </c>
       <c r="B28" s="8">
-        <v>0.27548209366391185</v>
+        <v>0.55529847292919943</v>
       </c>
       <c r="C28" s="8">
-        <v>0.2288329519450801</v>
+        <v>0</v>
       </c>
       <c r="D28" s="8">
         <v>2.766798418972332</v>
@@ -43929,10 +43931,10 @@
         <v>31</v>
       </c>
       <c r="B29" s="8">
-        <v>4.9586776859504136</v>
+        <v>4.8125867653863956</v>
       </c>
       <c r="C29" s="8">
-        <v>2.9748283752860414</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="D29" s="8">
         <v>13.043478260869565</v>
@@ -43959,10 +43961,10 @@
         <v>42</v>
       </c>
       <c r="B31" s="8">
-        <v>27.27272727272727</v>
+        <v>9.6251735307727913</v>
       </c>
       <c r="C31" s="8">
-        <v>17.391304347826086</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="D31" s="8">
         <v>9.8814229249011856</v>
@@ -43979,10 +43981,10 @@
         <v>43</v>
       </c>
       <c r="B32" s="8">
+        <v>6.5247570569180926</v>
+      </c>
+      <c r="C32" s="8">
         <v>3.0303030303030303</v>
-      </c>
-      <c r="C32" s="8">
-        <v>2.9748283752860414</v>
       </c>
       <c r="D32" s="8">
         <v>0.79051383399209485</v>
@@ -43999,10 +44001,10 @@
         <v>44</v>
       </c>
       <c r="B33" s="8">
-        <v>13.774104683195592</v>
+        <v>10.36557149467839</v>
       </c>
       <c r="C33" s="8">
-        <v>22.883295194508012</v>
+        <v>3.0303030303030303</v>
       </c>
       <c r="D33" s="8">
         <v>16.205533596837945</v>
@@ -44019,10 +44021,10 @@
         <v>45</v>
       </c>
       <c r="B34" s="8">
-        <v>5.785123966942149</v>
+        <v>66.496992133271632</v>
       </c>
       <c r="C34" s="8">
-        <v>4.3478260869565215</v>
+        <v>10.303030303030303</v>
       </c>
       <c r="D34" s="8">
         <v>1.1857707509881421</v>
@@ -44039,10 +44041,10 @@
         <v>46</v>
       </c>
       <c r="B35" s="8">
-        <v>4.4077134986225897</v>
+        <v>0.41647385469689957</v>
       </c>
       <c r="C35" s="8">
-        <v>4.1189931350114417</v>
+        <v>0</v>
       </c>
       <c r="D35" s="8">
         <v>5.1383399209486171</v>
@@ -44059,10 +44061,10 @@
         <v>47</v>
       </c>
       <c r="B36" s="8">
-        <v>30.303030303030305</v>
+        <v>3.7945395650161959</v>
       </c>
       <c r="C36" s="8">
-        <v>39.130434782608695</v>
+        <v>0</v>
       </c>
       <c r="D36" s="8">
         <v>35.573122529644266</v>
@@ -44079,10 +44081,10 @@
         <v>48</v>
       </c>
       <c r="B37" s="8">
-        <v>1.9283746556473829</v>
+        <v>2.4525682554372974</v>
       </c>
       <c r="C37" s="8">
-        <v>2.9748283752860414</v>
+        <v>1.8181818181818181</v>
       </c>
       <c r="D37" s="8">
         <v>0.79051383399209485</v>
@@ -44099,10 +44101,10 @@
         <v>49</v>
       </c>
       <c r="B38" s="8">
-        <v>1.6528925619834711</v>
+        <v>0.32392410920869968</v>
       </c>
       <c r="C38" s="8">
-        <v>1.3729977116704806</v>
+        <v>72.727272727272734</v>
       </c>
       <c r="D38" s="8">
         <v>1.1857707509881421</v>
@@ -44118,12 +44120,8 @@
       <c r="A39" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="8">
-        <v>1.1019283746556474</v>
-      </c>
-      <c r="C39" s="8">
-        <v>1.8306636155606408</v>
-      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="8">
         <v>0.79051383399209485</v>
       </c>
@@ -44139,10 +44137,10 @@
         <v>31</v>
       </c>
       <c r="B40" s="8">
-        <v>10.743801652892563</v>
+        <v>17.075428042572881</v>
       </c>
       <c r="C40" s="8">
-        <v>2.9748283752860414</v>
+        <v>6.0606060606060606</v>
       </c>
       <c r="D40" s="8">
         <v>28.458498023715418</v>
@@ -44158,8 +44156,12 @@
       <c r="A41" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="B41" s="8">
+        <v>0.64784821841739937</v>
+      </c>
+      <c r="C41" s="8">
+        <v>0.60606060606060608</v>
+      </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -44169,10 +44171,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="8">
-        <v>22.03856749311295</v>
+        <v>1.8047200370198981</v>
       </c>
       <c r="C42" s="8">
-        <v>22.883295194508012</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D42" s="8">
         <v>20.948616600790515</v>
@@ -44189,10 +44191,10 @@
         <v>142</v>
       </c>
       <c r="B43" s="8">
-        <v>15.702479338842975</v>
+        <v>1.4807959278111986</v>
       </c>
       <c r="C43" s="8">
-        <v>15.560640732265446</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D43" s="8">
         <v>17.391304347826086</v>
@@ -44209,10 +44211,10 @@
         <v>5</v>
       </c>
       <c r="B44" s="8">
-        <v>4.9586776859504136</v>
+        <v>5.9231837112447945</v>
       </c>
       <c r="C44" s="8">
-        <v>6.1784897025171626</v>
+        <v>2.4242424242424243</v>
       </c>
       <c r="D44" s="8">
         <v>4.7430830039525684</v>
@@ -44229,10 +44231,10 @@
         <v>143</v>
       </c>
       <c r="B45" s="8">
-        <v>7.1625344352617084</v>
+        <v>20.31466913465988</v>
       </c>
       <c r="C45" s="8">
-        <v>9.610983981693364</v>
+        <v>1.2121212121212122</v>
       </c>
       <c r="D45" s="8">
         <v>7.5098814229249005</v>
@@ -44249,10 +44251,10 @@
         <v>144</v>
       </c>
       <c r="B46" s="8">
-        <v>7.9889807162534439</v>
+        <v>11.568718186024988</v>
       </c>
       <c r="C46" s="8">
-        <v>5.4919908466819223</v>
+        <v>2.4242424242424243</v>
       </c>
       <c r="D46" s="8">
         <v>3.5573122529644272</v>
@@ -44269,10 +44271,10 @@
         <v>145</v>
       </c>
       <c r="B47" s="8">
-        <v>12.396694214876034</v>
+        <v>3.3780657103192966</v>
       </c>
       <c r="C47" s="8">
-        <v>11.441647597254006</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="D47" s="8">
         <v>5.1383399209486171</v>
@@ -44289,10 +44291,10 @@
         <v>146</v>
       </c>
       <c r="B48" s="8">
-        <v>10.46831955922865</v>
+        <v>9.254974548819991</v>
       </c>
       <c r="C48" s="8">
-        <v>15.331807780320366</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="D48" s="8">
         <v>9.8814229249011856</v>
@@ -44309,10 +44311,10 @@
         <v>31</v>
       </c>
       <c r="B49" s="8">
-        <v>19.28374655647383</v>
+        <v>28.227672373900969</v>
       </c>
       <c r="C49" s="8">
-        <v>13.501144164759726</v>
+        <v>6.0606060606060606</v>
       </c>
       <c r="D49" s="8">
         <v>30.830039525691699</v>
@@ -44328,8 +44330,12 @@
       <c r="A50" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
+      <c r="B50" s="8">
+        <v>0.32392410920869968</v>
+      </c>
+      <c r="C50" s="8">
+        <v>72.727272727272734</v>
+      </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -44338,12 +44344,8 @@
       <c r="A51" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="B51" s="8">
-        <v>34.435261707988978</v>
-      </c>
-      <c r="C51" s="8">
-        <v>38.901601830663616</v>
-      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
       <c r="D51" s="8">
         <v>25.691699604743086</v>
       </c>
@@ -44359,10 +44361,10 @@
         <v>149</v>
       </c>
       <c r="B52" s="8">
-        <v>46.005509641873275</v>
+        <v>20.31466913465988</v>
       </c>
       <c r="C52" s="8">
-        <v>51.716247139588098</v>
+        <v>10.303030303030303</v>
       </c>
       <c r="D52" s="8">
         <v>49.802371541501977</v>
@@ -44379,10 +44381,10 @@
         <v>31</v>
       </c>
       <c r="B53" s="8">
-        <v>19.55922865013774</v>
+        <v>79.68533086534012</v>
       </c>
       <c r="C53" s="8">
-        <v>9.3821510297482842</v>
+        <v>89.696969696969703</v>
       </c>
       <c r="D53" s="8">
         <v>24.505928853754941</v>
@@ -44398,17 +44400,19 @@
       <c r="A54" s="49" t="s">
         <v>150</v>
       </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="B55" s="8">
-        <v>83.746556473829202</v>
-      </c>
-      <c r="C55" s="8">
-        <v>80.320366132723109</v>
-      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
       <c r="D55" s="8">
         <v>84.980237154150188</v>
       </c>
@@ -44423,12 +44427,8 @@
       <c r="A56" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="8">
-        <v>15.977961432506888</v>
-      </c>
-      <c r="C56" s="8">
-        <v>19.679633867276888</v>
-      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="8">
         <v>15.019762845849801</v>
       </c>
@@ -44443,12 +44443,8 @@
       <c r="A57" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="8">
-        <v>0.27548209366391185</v>
-      </c>
-      <c r="C57" s="8">
-        <v>0</v>
-      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="8">
         <v>0</v>
       </c>
@@ -44463,51 +44459,211 @@
       <c r="A58" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="B58"/>
+      <c r="C58"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
         <v>51</v>
       </c>
+      <c r="B59"/>
+      <c r="C59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
         <v>52</v>
       </c>
+      <c r="B60"/>
+      <c r="C60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
         <v>53</v>
       </c>
+      <c r="B61"/>
+      <c r="C61"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
         <v>54</v>
       </c>
+      <c r="B62"/>
+      <c r="C62"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
         <v>55</v>
       </c>
+      <c r="B63"/>
+      <c r="C63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
         <v>56</v>
       </c>
+      <c r="B64"/>
+      <c r="C64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
         <v>57</v>
       </c>
+      <c r="B65"/>
+      <c r="C65"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
         <v>58</v>
       </c>
+      <c r="B66"/>
+      <c r="C66"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
         <v>59</v>
       </c>
+      <c r="B67"/>
+      <c r="C67"/>
+    </row>
+    <row r="68">
+      <c r="B68"/>
+      <c r="C68"/>
+    </row>
+    <row r="69">
+      <c r="B69"/>
+      <c r="C69"/>
+    </row>
+    <row r="70">
+      <c r="B70"/>
+      <c r="C70"/>
+    </row>
+    <row r="71">
+      <c r="B71"/>
+      <c r="C71"/>
+    </row>
+    <row r="72">
+      <c r="B72"/>
+      <c r="C72"/>
+    </row>
+    <row r="73">
+      <c r="B73"/>
+      <c r="C73"/>
+    </row>
+    <row r="74">
+      <c r="B74"/>
+      <c r="C74"/>
+    </row>
+    <row r="75">
+      <c r="B75"/>
+      <c r="C75"/>
+    </row>
+    <row r="76">
+      <c r="B76"/>
+      <c r="C76"/>
+    </row>
+    <row r="77">
+      <c r="B77"/>
+      <c r="C77"/>
+    </row>
+    <row r="78">
+      <c r="B78"/>
+      <c r="C78"/>
+    </row>
+    <row r="79">
+      <c r="B79"/>
+      <c r="C79"/>
+    </row>
+    <row r="80">
+      <c r="B80"/>
+      <c r="C80"/>
+    </row>
+    <row r="81">
+      <c r="B81"/>
+      <c r="C81"/>
+    </row>
+    <row r="82">
+      <c r="B82"/>
+      <c r="C82"/>
+    </row>
+    <row r="83">
+      <c r="B83"/>
+      <c r="C83"/>
+    </row>
+    <row r="84">
+      <c r="B84"/>
+      <c r="C84"/>
+    </row>
+    <row r="85">
+      <c r="B85"/>
+      <c r="C85"/>
+    </row>
+    <row r="86">
+      <c r="B86"/>
+      <c r="C86"/>
+    </row>
+    <row r="87">
+      <c r="B87"/>
+      <c r="C87"/>
+    </row>
+    <row r="88">
+      <c r="B88"/>
+      <c r="C88"/>
+    </row>
+    <row r="89">
+      <c r="B89"/>
+      <c r="C89"/>
+    </row>
+    <row r="90">
+      <c r="B90"/>
+      <c r="C90"/>
+    </row>
+    <row r="91">
+      <c r="B91"/>
+      <c r="C91"/>
+    </row>
+    <row r="92">
+      <c r="B92"/>
+      <c r="C92"/>
+    </row>
+    <row r="93">
+      <c r="B93"/>
+      <c r="C93"/>
+    </row>
+    <row r="94">
+      <c r="B94"/>
+      <c r="C94"/>
+    </row>
+    <row r="95">
+      <c r="B95"/>
+      <c r="C95"/>
+    </row>
+    <row r="96">
+      <c r="B96"/>
+      <c r="C96"/>
+    </row>
+    <row r="97">
+      <c r="B97"/>
+      <c r="C97"/>
+    </row>
+    <row r="98">
+      <c r="B98"/>
+      <c r="C98"/>
+    </row>
+    <row r="99">
+      <c r="B99"/>
+      <c r="C99"/>
+    </row>
+    <row r="100">
+      <c r="B100"/>
+      <c r="C100"/>
+    </row>
+    <row r="101">
+      <c r="B101"/>
+      <c r="C101"/>
+    </row>
+    <row r="102">
+      <c r="B102"/>
+      <c r="C102"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>